<commit_message>
locked left columns and updated overall impression
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="602">
   <si>
     <t xml:space="preserve">Metrics &amp; Description</t>
   </si>
@@ -729,25 +729,7 @@
     <t xml:space="preserve">yes, optimization mentioned in User Guide</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, parallelism among other things described in </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/aharwood2/LUMA/wiki/Performance</t>
-    </r>
+    <t xml:space="preserve">yes, parallelism among other things described in https://github.com/aharwood2/LUMA/wiki/Performance</t>
   </si>
   <si>
     <t xml:space="preserve">yes, parallel build available</t>
@@ -864,25 +846,7 @@
     <t xml:space="preserve">yes, tutorial package</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, installation has a command to run the program; there is also </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/aharwood2/LUMA/wiki/Validation</t>
-    </r>
+    <t xml:space="preserve">yes, installation has a command to run the program; there is also https://github.com/aharwood2/LUMA/wiki/Validation</t>
   </si>
   <si>
     <t xml:space="preserve">yes, there is a make test that can be run after the installation</t>
@@ -1056,67 +1020,13 @@
     <t xml:space="preserve">({yes∗ , no, unclear})</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, some theory in publications and documentations on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://walberla.net/index.html</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://sunlightlb.sourceforge.net/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://sailfish.us.edu.pl/media.html#academic-papers</t>
-    </r>
+    <t xml:space="preserve">yes, some theory in publications and documentations on https://walberla.net/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, http://sunlightlb.sourceforge.net/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, http://sailfish.us.edu.pl/media.html#academic-papers</t>
   </si>
   <si>
     <t xml:space="preserve">yes, in the user guide</t>
@@ -1125,25 +1035,7 @@
     <t xml:space="preserve">yes, some theory in user guide</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, link to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/aharwood2/LUMA/wiki</t>
-    </r>
+    <t xml:space="preserve">yes, link to https://github.com/aharwood2/LUMA/wiki</t>
   </si>
   <si>
     <t xml:space="preserve">yes, reference document https://github.com/ludwig-cf/ludwig/blob/master/docs/references.tex</t>
@@ -1424,25 +1316,7 @@
     <t xml:space="preserve">Are expected user characteristics documented?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, in </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://palabos.unige.ch/</t>
-    </r>
+    <t xml:space="preserve">yes, in https://palabos.unige.ch/</t>
   </si>
   <si>
     <t xml:space="preserve">What is the user support model? FAQ? User forum? E-mail address to direct questions? Etc.</t>
@@ -1535,67 +1409,13 @@
     <t xml:space="preserve">Is there any information on how code is reviewed, or how to contribute?</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://i10git.cs.fau.de/walberla/walberla</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://sailfish.us.edu.pl/about.html#development-team</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://gitlab.com/unigespc/palabos/blob/master/CONTRIBUTING.md</t>
-    </r>
+    <t xml:space="preserve">yes, https://i10git.cs.fau.de/walberla/walberla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, http://sailfish.us.edu.pl/about.html#development-team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, https://gitlab.com/unigespc/palabos/blob/master/CONTRIBUTING.md</t>
   </si>
   <si>
     <t xml:space="preserve">yes, developer guide</t>
@@ -1790,25 +1610,7 @@
     <t xml:space="preserve">({yes∗, no, n/a})</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/aharwood2/LUMA/blob/master/LUMA/docs/LUMA%20Coding%20Standards.pdf</t>
-    </r>
+    <t xml:space="preserve">yes, https://github.com/aharwood2/LUMA/blob/master/LUMA/docs/LUMA%20Coding%20Standards.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">yes, found in hemelbCodingStandard.txt</t>
@@ -1874,25 +1676,7 @@
     <t xml:space="preserve">Are there any documents recording the development process and status? </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://gitlab.com/unigespc/palabos/-/blob/master/CONTRIBUTING.md</t>
-    </r>
+    <t xml:space="preserve">yes, https://gitlab.com/unigespc/palabos/-/blob/master/CONTRIBUTING.md</t>
   </si>
   <si>
     <t xml:space="preserve">yes, in https://github.com/ludwig-cf/ludwig/blob/master/CONTRIBUTING.md</t>
@@ -1937,94 +1721,19 @@
     <t xml:space="preserve">Are there release notes? </t>
   </si>
   <si>
-    <t xml:space="preserve">yes, https://i10git.cs.fau.de/walberla/walberla</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://sailfish.us.edu.pl/release.html</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://gitlab.com/unigespc/palabos/-/blob/master/CHANGELOG.md</t>
-    </r>
+    <t xml:space="preserve">yes, http://sailfish.us.edu.pl/release.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, https://gitlab.com/unigespc/palabos/-/blob/master/CHANGELOG.md</t>
   </si>
   <si>
     <t xml:space="preserve">yes, in downloads page</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/carlosrosales/mplabs/blob/master/CHANGES.TXT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">yes, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/aharwood2/LUMA/wiki/Release-Notes</t>
-    </r>
+    <t xml:space="preserve">yes, https://github.com/carlosrosales/mplabs/blob/master/CHANGES.TXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, https://github.com/aharwood2/LUMA/wiki/Release-Notes</t>
   </si>
   <si>
     <t xml:space="preserve">yes, README is updates alongside releases</t>
@@ -2211,7 +1920,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2242,11 +1951,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2257,6 +1961,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2328,7 +2033,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2365,15 +2070,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2395,6 +2096,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2432,13 +2149,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="V91" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
+      <selection pane="topRight" activeCell="W102" activeCellId="0" sqref="W102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -2580,19 +2297,19 @@
       <c r="F4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
@@ -2607,7 +2324,7 @@
       <c r="O4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="8" t="s">
         <v>43</v>
       </c>
       <c r="Q4" s="7" t="s">
@@ -2616,19 +2333,19 @@
       <c r="R4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="9" t="s">
         <v>49</v>
       </c>
       <c r="X4" s="7" t="s">
@@ -2648,7 +2365,7 @@
       <c r="D5" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -2725,7 +2442,7 @@
       <c r="E6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -3012,40 +2729,40 @@
       <c r="B10" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="11" t="n">
         <v>39661</v>
       </c>
-      <c r="D10" s="12" t="n">
+      <c r="D10" s="11" t="n">
         <v>38597</v>
       </c>
-      <c r="E10" s="12" t="n">
+      <c r="E10" s="11" t="n">
         <v>41196</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G10" s="12" t="n">
+      <c r="G10" s="11" t="n">
         <v>39280</v>
       </c>
-      <c r="H10" s="12" t="n">
+      <c r="H10" s="11" t="n">
         <v>39614</v>
       </c>
-      <c r="I10" s="12" t="n">
+      <c r="I10" s="11" t="n">
         <v>39607</v>
       </c>
-      <c r="J10" s="12" t="n">
+      <c r="J10" s="11" t="n">
         <v>42676</v>
       </c>
-      <c r="K10" s="12" t="n">
+      <c r="K10" s="11" t="n">
         <v>43314</v>
       </c>
-      <c r="L10" s="12" t="n">
+      <c r="L10" s="11" t="n">
         <v>40503</v>
       </c>
-      <c r="M10" s="12" t="n">
+      <c r="M10" s="11" t="n">
         <v>43592</v>
       </c>
-      <c r="N10" s="12" t="n">
+      <c r="N10" s="11" t="n">
         <v>42185</v>
       </c>
       <c r="O10" s="7" t="s">
@@ -3063,19 +2780,19 @@
       <c r="S10" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="T10" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="U10" s="14" t="n">
+      <c r="U10" s="13" t="n">
         <v>40489</v>
       </c>
-      <c r="V10" s="14" t="n">
+      <c r="V10" s="13" t="n">
         <v>40598</v>
       </c>
-      <c r="W10" s="14" t="n">
+      <c r="W10" s="13" t="n">
         <v>39260</v>
       </c>
-      <c r="X10" s="14" t="n">
+      <c r="X10" s="13" t="n">
         <v>41953</v>
       </c>
     </row>
@@ -3086,70 +2803,70 @@
       <c r="B11" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="11" t="n">
         <v>44025</v>
       </c>
-      <c r="D11" s="12" t="n">
+      <c r="D11" s="11" t="n">
         <v>41234</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="E11" s="11" t="n">
         <v>43627</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="11" t="n">
         <v>44023</v>
       </c>
-      <c r="G11" s="12" t="n">
+      <c r="G11" s="11" t="n">
         <v>43727</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="11" t="n">
         <v>41928</v>
       </c>
-      <c r="I11" s="12" t="n">
+      <c r="I11" s="11" t="n">
         <v>44014</v>
       </c>
-      <c r="J11" s="12" t="n">
+      <c r="J11" s="11" t="n">
         <v>43874</v>
       </c>
-      <c r="K11" s="12" t="n">
+      <c r="K11" s="11" t="n">
         <v>44020</v>
       </c>
-      <c r="L11" s="12" t="n">
+      <c r="L11" s="11" t="n">
         <v>41974</v>
       </c>
-      <c r="M11" s="12" t="n">
+      <c r="M11" s="11" t="n">
         <v>44018</v>
       </c>
-      <c r="N11" s="12" t="n">
+      <c r="N11" s="11" t="n">
         <v>44011</v>
       </c>
-      <c r="O11" s="12" t="n">
+      <c r="O11" s="11" t="n">
         <v>44012</v>
       </c>
-      <c r="P11" s="12" t="n">
+      <c r="P11" s="11" t="n">
         <v>40980</v>
       </c>
-      <c r="Q11" s="12" t="n">
+      <c r="Q11" s="11" t="n">
         <v>40835</v>
       </c>
-      <c r="R11" s="12" t="n">
+      <c r="R11" s="11" t="n">
         <v>41017</v>
       </c>
-      <c r="S11" s="12" t="n">
+      <c r="S11" s="11" t="n">
         <v>42790</v>
       </c>
-      <c r="T11" s="15" t="n">
+      <c r="T11" s="14" t="n">
         <v>43922</v>
       </c>
-      <c r="U11" s="14" t="n">
+      <c r="U11" s="13" t="n">
         <v>44004</v>
       </c>
-      <c r="V11" s="14" t="n">
+      <c r="V11" s="13" t="n">
         <v>43943</v>
       </c>
-      <c r="W11" s="14" t="n">
+      <c r="W11" s="13" t="n">
         <v>43322</v>
       </c>
-      <c r="X11" s="14" t="n">
+      <c r="X11" s="13" t="n">
         <v>43339</v>
       </c>
     </row>
@@ -3523,7 +3240,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" s="16" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>159</v>
       </c>
@@ -3581,19 +3298,19 @@
       <c r="S17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="T17" s="16" t="n">
+      <c r="T17" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="U17" s="16" t="n">
+      <c r="U17" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="V17" s="16" t="n">
+      <c r="V17" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="W17" s="16" t="n">
+      <c r="W17" s="15" t="n">
         <v>221</v>
       </c>
-      <c r="X17" s="16" t="n">
+      <c r="X17" s="15" t="n">
         <v>7</v>
       </c>
       <c r="AMJ17" s="0"/>
@@ -3623,10 +3340,10 @@
       <c r="H18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="8" t="s">
         <v>170</v>
       </c>
       <c r="K18" s="7" t="s">
@@ -3641,10 +3358,10 @@
       <c r="N18" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="O18" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="8" t="s">
         <v>175</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -3656,16 +3373,16 @@
       <c r="S18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="U18" s="10" t="s">
+      <c r="U18" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="V18" s="10" t="s">
+      <c r="V18" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="W18" s="10" t="s">
+      <c r="W18" s="9" t="s">
         <v>182</v>
       </c>
       <c r="X18" s="7" t="s">
@@ -3774,7 +3491,7 @@
       <c r="I20" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="8" t="s">
         <v>214</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3813,7 +3530,7 @@
       <c r="V20" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="W20" s="10" t="s">
+      <c r="W20" s="9" t="s">
         <v>223</v>
       </c>
       <c r="X20" s="0" t="s">
@@ -4239,299 +3956,299 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+    <row r="28" s="18" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="N28" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="P28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="R28" s="1" t="s">
+      <c r="R28" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="S28" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="T28" s="0" t="s">
+      <c r="S28" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="T28" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="U28" s="0" t="s">
+      <c r="U28" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="V28" s="0" t="s">
+      <c r="V28" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="W28" s="0" t="s">
+      <c r="W28" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="X28" s="0" t="s">
+      <c r="X28" s="17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+    <row r="29" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="C29" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="7" t="s">
+      <c r="H29" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="J29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="L29" s="7" t="s">
+      <c r="J29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="M29" s="7" t="s">
+      <c r="M29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="N29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q29" s="7" t="s">
+      <c r="N29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="O29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="P29" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="R29" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="T29" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="U29" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="V29" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="W29" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="X29" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="R29" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="S29" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="T29" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="U29" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="V29" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="W29" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="X29" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" s="18" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L30" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="N30" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="O30" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="P30" s="1" t="s">
+      <c r="O30" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="P30" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="Q30" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="R30" s="1" t="s">
+      <c r="Q30" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="R30" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="S30" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="T30" s="0" t="s">
+      <c r="T30" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="U30" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="V30" s="7" t="s">
+      <c r="U30" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="V30" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="W30" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="X30" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="W30" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="X30" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" s="18" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="E31" s="7" t="n">
+      <c r="E31" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="F31" s="7" t="n">
+      <c r="F31" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="G31" s="7" t="n">
+      <c r="G31" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="7" t="n">
+      <c r="H31" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="J31" s="7" t="n">
+      <c r="J31" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="K31" s="7" t="n">
+      <c r="K31" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="L31" s="7" t="n">
+      <c r="L31" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="M31" s="7" t="n">
+      <c r="M31" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="N31" s="7" t="n">
+      <c r="N31" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="O31" s="7" t="s">
+      <c r="O31" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="P31" s="7" t="n">
+      <c r="P31" s="16" t="n">
         <v>13</v>
       </c>
-      <c r="Q31" s="7" t="n">
+      <c r="Q31" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="R31" s="7" t="s">
+      <c r="R31" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="S31" s="7" t="s">
+      <c r="S31" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="T31" s="0" t="s">
+      <c r="T31" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="U31" s="0" t="s">
+      <c r="U31" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="V31" s="0" t="s">
+      <c r="V31" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="W31" s="0" t="s">
+      <c r="W31" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="X31" s="0" t="s">
+      <c r="X31" s="17" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4913,19 +4630,19 @@
         <v>287</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1" t="n">
         <v>9</v>
       </c>
       <c r="G37" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37" s="1" t="n">
         <v>6</v>
@@ -4934,37 +4651,37 @@
         <v>10</v>
       </c>
       <c r="J37" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K37" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L37" s="1" t="n">
         <v>8</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N37" s="1" t="n">
         <v>8</v>
       </c>
       <c r="O37" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P37" s="1" t="n">
         <v>8</v>
       </c>
       <c r="Q37" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="R37" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S37" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T37" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U37" s="0" t="n">
         <v>9</v>
@@ -4973,10 +4690,10 @@
         <v>5</v>
       </c>
       <c r="W37" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X37" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5032,7 +4749,7 @@
       <c r="R38" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="S38" s="9" t="s">
+      <c r="S38" s="8" t="s">
         <v>304</v>
       </c>
       <c r="V38" s="7" t="s">
@@ -5076,13 +4793,13 @@
       <c r="B40" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="8" t="s">
         <v>313</v>
       </c>
       <c r="F40" s="7" t="s">
@@ -5097,19 +4814,19 @@
       <c r="I40" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="J40" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="K40" s="9" t="s">
+      <c r="K40" s="8" t="s">
         <v>317</v>
       </c>
       <c r="L40" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N40" s="8" t="s">
         <v>319</v>
       </c>
       <c r="O40" s="7" t="s">
@@ -5136,7 +4853,7 @@
       <c r="V40" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="W40" s="10" t="s">
+      <c r="W40" s="9" t="s">
         <v>323</v>
       </c>
       <c r="X40" s="0" t="s">
@@ -5669,7 +5386,7 @@
         <v>287</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>2</v>
@@ -5678,34 +5395,34 @@
         <v>6</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G48" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H48" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J48" s="1" t="n">
         <v>6</v>
       </c>
       <c r="K48" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L48" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M48" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N48" s="1" t="n">
         <v>8</v>
       </c>
       <c r="O48" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P48" s="1" t="n">
         <v>6</v>
@@ -5714,19 +5431,19 @@
         <v>2</v>
       </c>
       <c r="R48" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S48" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U48" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="V48" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="U48" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="V48" s="0" t="n">
-        <v>6</v>
       </c>
       <c r="W48" s="0" t="n">
         <v>2</v>
@@ -6180,13 +5897,13 @@
         <v>287</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F56" s="1" t="n">
         <v>10</v>
@@ -6195,19 +5912,19 @@
         <v>10</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="1" t="n">
         <v>10</v>
       </c>
       <c r="J56" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K56" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L56" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M56" s="1" t="n">
         <v>10</v>
@@ -6216,31 +5933,31 @@
         <v>10</v>
       </c>
       <c r="O56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S56" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T56" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U56" s="0" t="n">
         <v>10</v>
       </c>
       <c r="V56" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W56" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X56" s="0" t="n">
         <v>10</v>
@@ -6308,7 +6025,7 @@
       <c r="S58" s="5"/>
       <c r="AMJ58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="60.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>387</v>
       </c>
@@ -6464,13 +6181,13 @@
         <v>287</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E61" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F61" s="1" t="n">
         <v>10</v>
@@ -6500,16 +6217,16 @@
         <v>10</v>
       </c>
       <c r="O61" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q61" s="1" t="n">
         <v>10</v>
       </c>
       <c r="R61" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S61" s="1" t="n">
         <v>0</v>
@@ -6521,10 +6238,10 @@
         <v>10</v>
       </c>
       <c r="V61" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="W61" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="W61" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="X61" s="0" t="n">
         <v>10</v>
@@ -6750,7 +6467,7 @@
       <c r="E66" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" s="8" t="s">
         <v>404</v>
       </c>
       <c r="G66" s="1" t="s">
@@ -6890,55 +6607,55 @@
         <v>287</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F68" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G68" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J68" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="F68" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="G68" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H68" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I68" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J68" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="K68" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L68" s="1" t="n">
         <v>4</v>
       </c>
       <c r="M68" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N68" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O68" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P68" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q68" s="1" t="n">
         <v>5</v>
       </c>
       <c r="R68" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S68" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T68" s="0" t="n">
         <v>8</v>
@@ -6950,7 +6667,7 @@
         <v>8</v>
       </c>
       <c r="W68" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X68" s="0" t="n">
         <v>9</v>
@@ -6973,7 +6690,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
-      <c r="K69" s="9" t="s">
+      <c r="K69" s="8" t="s">
         <v>416</v>
       </c>
       <c r="L69" s="2"/>
@@ -7076,10 +6793,10 @@
       <c r="T71" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="U71" s="17" t="s">
+      <c r="U71" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="V71" s="17" t="s">
+      <c r="V71" s="20" t="s">
         <v>431</v>
       </c>
       <c r="W71" s="0" t="s">
@@ -7096,16 +6813,16 @@
       <c r="B72" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="8" t="s">
         <v>435</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="8" t="s">
         <v>437</v>
       </c>
       <c r="G72" s="7" t="s">
@@ -7120,13 +6837,13 @@
       <c r="J72" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="K72" s="9" t="s">
+      <c r="K72" s="8" t="s">
         <v>440</v>
       </c>
       <c r="L72" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="M72" s="9" t="s">
+      <c r="M72" s="8" t="s">
         <v>441</v>
       </c>
       <c r="N72" s="7" t="s">
@@ -7318,40 +7035,40 @@
       <c r="B75" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C75" s="18" t="n">
+      <c r="C75" s="21" t="n">
         <v>0.729</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E75" s="18" t="n">
+      <c r="E75" s="21" t="n">
         <v>0.2222</v>
       </c>
-      <c r="F75" s="18" t="n">
+      <c r="F75" s="21" t="n">
         <v>0.8947</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="H75" s="18" t="n">
+      <c r="H75" s="21" t="n">
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="J75" s="18" t="n">
+      <c r="J75" s="21" t="n">
         <v>0.8571</v>
       </c>
-      <c r="K75" s="18" t="n">
+      <c r="K75" s="21" t="n">
         <v>0.6</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="M75" s="18" t="n">
+      <c r="M75" s="21" t="n">
         <v>0.3333</v>
       </c>
-      <c r="N75" s="18" t="n">
+      <c r="N75" s="21" t="n">
         <v>0.6666</v>
       </c>
       <c r="O75" s="1" t="s">
@@ -7366,22 +7083,22 @@
       <c r="R75" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="S75" s="18" t="n">
+      <c r="S75" s="21" t="n">
         <v>0.9333</v>
       </c>
-      <c r="T75" s="19" t="n">
+      <c r="T75" s="22" t="n">
         <v>0.6032</v>
       </c>
-      <c r="U75" s="19" t="n">
+      <c r="U75" s="22" t="n">
         <v>0.8926</v>
       </c>
-      <c r="V75" s="19" t="n">
+      <c r="V75" s="22" t="n">
         <v>0.6628</v>
       </c>
       <c r="W75" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="X75" s="19" t="n">
+      <c r="X75" s="22" t="n">
         <v>0.1875</v>
       </c>
     </row>
@@ -7392,72 +7109,73 @@
       <c r="B76" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="C76" s="20" t="n">
+      <c r="C76" s="23" t="n">
         <v>0.2262</v>
       </c>
-      <c r="D76" s="20" t="n">
+      <c r="D76" s="23" t="n">
         <v>0.1767</v>
       </c>
-      <c r="E76" s="20" t="n">
+      <c r="E76" s="23" t="n">
         <v>0.0926</v>
       </c>
-      <c r="F76" s="20" t="n">
+      <c r="F76" s="23" t="n">
         <v>0.1776</v>
       </c>
-      <c r="G76" s="20" t="n">
+      <c r="G76" s="23" t="n">
         <v>0.2243</v>
       </c>
-      <c r="H76" s="20" t="n">
+      <c r="H76" s="23" t="n">
         <v>0.2667</v>
       </c>
-      <c r="I76" s="20" t="n">
+      <c r="I76" s="23" t="n">
         <v>0.1511</v>
       </c>
-      <c r="J76" s="20" t="n">
+      <c r="J76" s="23" t="n">
         <v>0.002</v>
       </c>
-      <c r="K76" s="20" t="n">
+      <c r="K76" s="23" t="n">
         <v>0.207</v>
       </c>
-      <c r="L76" s="20" t="n">
+      <c r="L76" s="23" t="n">
         <v>0.1739</v>
       </c>
-      <c r="M76" s="20" t="n">
+      <c r="M76" s="23" t="n">
         <v>0.0819</v>
       </c>
-      <c r="N76" s="20" t="n">
+      <c r="N76" s="23" t="n">
         <v>0.1612</v>
       </c>
-      <c r="O76" s="20" t="n">
+      <c r="O76" s="23" t="n">
         <v>0.0203</v>
       </c>
-      <c r="P76" s="20" t="n">
+      <c r="P76" s="23" t="n">
         <v>0.1376</v>
       </c>
-      <c r="Q76" s="20" t="n">
+      <c r="Q76" s="23" t="n">
         <v>0.1361</v>
       </c>
-      <c r="R76" s="20" t="n">
+      <c r="R76" s="23" t="n">
         <v>0.1434</v>
       </c>
-      <c r="S76" s="20" t="n">
+      <c r="S76" s="23" t="n">
         <v>0.004</v>
       </c>
-      <c r="T76" s="19" t="n">
+      <c r="T76" s="22" t="n">
         <v>0.0602</v>
       </c>
-      <c r="U76" s="19" t="n">
+      <c r="U76" s="22" t="n">
         <v>0.2178</v>
       </c>
-      <c r="V76" s="19" t="n">
+      <c r="V76" s="22" t="n">
         <v>0.171</v>
       </c>
-      <c r="W76" s="19" t="n">
+      <c r="W76" s="22" t="n">
         <v>0.1668</v>
       </c>
-      <c r="X76" s="19" t="n">
+      <c r="X76" s="22" t="n">
         <v>0.0247</v>
       </c>
+      <c r="AB76" s="22"/>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
@@ -7544,67 +7262,67 @@
         <v>10</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="F78" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F78" s="1" t="n">
+      <c r="G78" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H78" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J78" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K78" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L78" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M78" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="G78" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="H78" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I78" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J78" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="K78" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="L78" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M78" s="1" t="n">
+      <c r="N78" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="N78" s="1" t="n">
-        <v>7</v>
       </c>
       <c r="O78" s="1" t="n">
         <v>6</v>
       </c>
       <c r="P78" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q78" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R78" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S78" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T78" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U78" s="0" t="n">
         <v>10</v>
       </c>
       <c r="V78" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="W78" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X78" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="W78" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="X78" s="0" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7657,7 +7375,7 @@
       <c r="S80" s="5"/>
       <c r="AMJ80" s="0"/>
     </row>
-    <row r="81" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7" t="s">
         <v>494</v>
       </c>
@@ -7715,19 +7433,19 @@
       <c r="S81" s="7" t="n">
         <v>41</v>
       </c>
-      <c r="T81" s="16" t="n">
+      <c r="T81" s="15" t="n">
         <v>542</v>
       </c>
-      <c r="U81" s="16" t="n">
+      <c r="U81" s="15" t="n">
         <v>1395</v>
       </c>
-      <c r="V81" s="16" t="n">
+      <c r="V81" s="15" t="n">
         <v>5394</v>
       </c>
-      <c r="W81" s="16" t="n">
+      <c r="W81" s="15" t="n">
         <v>1113</v>
       </c>
-      <c r="X81" s="16" t="n">
+      <c r="X81" s="15" t="n">
         <v>134</v>
       </c>
       <c r="AMJ81" s="0"/>
@@ -7817,16 +7535,16 @@
         <v>10</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F83" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G83" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H83" s="1" t="n">
         <v>5</v>
@@ -7838,46 +7556,46 @@
         <v>5</v>
       </c>
       <c r="K83" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M83" s="1" t="n">
         <v>5</v>
-      </c>
-      <c r="L83" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M83" s="1" t="n">
-        <v>8</v>
       </c>
       <c r="N83" s="1" t="n">
         <v>5</v>
       </c>
       <c r="O83" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P83" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q83" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R83" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S83" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T83" s="0" t="n">
         <v>5</v>
       </c>
       <c r="U83" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="V83" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="V83" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="W83" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="X83" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="35.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7895,7 +7613,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
-      <c r="M84" s="9" t="s">
+      <c r="M84" s="8" t="s">
         <v>497</v>
       </c>
       <c r="N84" s="2"/>
@@ -8031,7 +7749,7 @@
       <c r="I87" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="J87" s="1" t="s">
+      <c r="J87" s="8" t="s">
         <v>502</v>
       </c>
       <c r="K87" s="1" t="s">
@@ -8164,16 +7882,16 @@
       <c r="D89" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E89" s="7" t="s">
         <v>507</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G89" s="8" t="s">
+      <c r="G89" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="H89" s="8" t="s">
+      <c r="H89" s="7" t="s">
         <v>507</v>
       </c>
       <c r="I89" s="7" t="s">
@@ -8535,13 +8253,13 @@
         <v>8</v>
       </c>
       <c r="E94" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F94" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G94" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H94" s="1" t="n">
         <v>5</v>
@@ -8553,7 +8271,7 @@
         <v>10</v>
       </c>
       <c r="K94" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L94" s="1" t="n">
         <v>5</v>
@@ -8562,34 +8280,34 @@
         <v>9</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O94" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q94" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R94" s="1" t="n">
         <v>6</v>
       </c>
       <c r="S94" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="T94" s="0" t="n">
         <v>8</v>
       </c>
       <c r="U94" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="V94" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="W94" s="0" t="n">
         <v>8</v>
-      </c>
-      <c r="V94" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="W94" s="0" t="n">
-        <v>9</v>
       </c>
       <c r="X94" s="0" t="n">
         <v>8</v>
@@ -8670,7 +8388,7 @@
       <c r="J97" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="K97" s="9" t="s">
+      <c r="K97" s="8" t="s">
         <v>522</v>
       </c>
       <c r="L97" s="7" t="s">
@@ -8729,7 +8447,7 @@
       <c r="E98" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="F98" s="7" t="s">
+      <c r="F98" s="8" t="s">
         <v>524</v>
       </c>
       <c r="G98" s="7" t="s">
@@ -8744,7 +8462,7 @@
       <c r="J98" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="K98" s="9" t="s">
+      <c r="K98" s="8" t="s">
         <v>525</v>
       </c>
       <c r="L98" s="7" t="s">
@@ -8753,10 +8471,10 @@
       <c r="M98" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="N98" s="9" t="s">
+      <c r="N98" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="O98" s="9" t="s">
+      <c r="O98" s="8" t="s">
         <v>527</v>
       </c>
       <c r="P98" s="7" t="s">
@@ -8821,10 +8539,10 @@
       <c r="K99" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="L99" s="9" t="s">
+      <c r="L99" s="8" t="s">
         <v>533</v>
       </c>
-      <c r="M99" s="9" t="s">
+      <c r="M99" s="8" t="s">
         <v>534</v>
       </c>
       <c r="N99" s="7" t="s">
@@ -8842,7 +8560,7 @@
       <c r="R99" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="S99" s="9" t="s">
+      <c r="S99" s="8" t="s">
         <v>536</v>
       </c>
       <c r="T99" s="0" t="s">
@@ -8869,31 +8587,31 @@
         <v>208</v>
       </c>
       <c r="C100" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="D100" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E100" s="7" t="s">
+      <c r="F100" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="F100" s="7" t="s">
+      <c r="G100" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="G100" s="7" t="s">
+      <c r="H100" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="H100" s="7" t="s">
+      <c r="I100" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J100" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="I100" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="J100" s="7" t="s">
+      <c r="K100" s="7" t="s">
         <v>544</v>
-      </c>
-      <c r="K100" s="7" t="s">
-        <v>545</v>
       </c>
       <c r="L100" s="7" t="s">
         <v>210</v>
@@ -8949,61 +8667,61 @@
         <v>0</v>
       </c>
       <c r="E101" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F101" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G101" s="1" t="n">
         <v>4</v>
       </c>
       <c r="H101" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I101" s="1" t="n">
         <v>0</v>
       </c>
       <c r="J101" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K101" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N101" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="M101" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="N101" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="O101" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P101" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="T101" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U101" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="R101" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="S101" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="T101" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="U101" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="V101" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W101" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X101" s="0" t="n">
         <v>0</v>
@@ -9015,7 +8733,7 @@
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -9026,8 +8744,8 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
-      <c r="M102" s="9" t="s">
-        <v>547</v>
+      <c r="M102" s="8" t="s">
+        <v>546</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
@@ -9038,7 +8756,7 @@
     </row>
     <row r="105" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
@@ -9054,7 +8772,7 @@
       <c r="M105" s="5"/>
       <c r="N105" s="5"/>
       <c r="O105" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P105" s="5"/>
       <c r="Q105" s="5"/>
@@ -9064,7 +8782,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>94</v>
@@ -9138,7 +8856,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>94</v>
@@ -9212,7 +8930,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>94</v>
@@ -9286,7 +9004,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>94</v>
@@ -9295,7 +9013,7 @@
         <v>1573654</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E109" s="7" t="n">
         <v>154310</v>
@@ -9304,13 +9022,13 @@
         <v>727494</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H109" s="7" t="n">
         <v>192269</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J109" s="7" t="n">
         <v>10725979</v>
@@ -9319,7 +9037,7 @@
         <v>2252783</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M109" s="7" t="n">
         <v>6322</v>
@@ -9331,7 +9049,7 @@
         <v>89081</v>
       </c>
       <c r="P109" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q109" s="7" t="n">
         <v>16078</v>
@@ -9360,7 +9078,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>94</v>
@@ -9369,7 +9087,7 @@
         <v>297209</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E110" s="7" t="n">
         <v>71872</v>
@@ -9378,13 +9096,13 @@
         <v>173808</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H110" s="7" t="n">
         <v>149144</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J110" s="7" t="n">
         <v>5201357</v>
@@ -9393,7 +9111,7 @@
         <v>1580570</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M110" s="7" t="n">
         <v>740</v>
@@ -9405,7 +9123,7 @@
         <v>42448</v>
       </c>
       <c r="P110" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q110" s="7" t="n">
         <v>3132</v>
@@ -9434,7 +9152,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>94</v>
@@ -9443,7 +9161,7 @@
         <v>1314</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E111" s="7" t="n">
         <v>1846</v>
@@ -9452,13 +9170,13 @@
         <v>132</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H111" s="7" t="n">
         <v>11</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J111" s="7" t="n">
         <v>697</v>
@@ -9467,7 +9185,7 @@
         <v>2059</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M111" s="7" t="n">
         <v>50</v>
@@ -9479,7 +9197,7 @@
         <v>488</v>
       </c>
       <c r="P111" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q111" s="7" t="n">
         <v>14</v>
@@ -9508,52 +9226,52 @@
     </row>
     <row r="112" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="D112" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E112" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="E112" s="7" t="s">
+      <c r="F112" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="F112" s="7" t="s">
-        <v>562</v>
-      </c>
       <c r="G112" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H112" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I112" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="K112" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="M112" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="N112" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="O112" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="P112" s="7" t="s">
         <v>554</v>
-      </c>
-      <c r="J112" s="7" t="s">
-        <v>563</v>
-      </c>
-      <c r="K112" s="7" t="s">
-        <v>564</v>
-      </c>
-      <c r="L112" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="M112" s="7" t="s">
-        <v>565</v>
-      </c>
-      <c r="N112" s="7" t="s">
-        <v>566</v>
-      </c>
-      <c r="O112" s="7" t="s">
-        <v>567</v>
-      </c>
-      <c r="P112" s="7" t="s">
-        <v>555</v>
       </c>
       <c r="Q112" s="7" t="n">
         <v>0</v>
@@ -9562,70 +9280,70 @@
         <v>0</v>
       </c>
       <c r="S112" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="T112" s="0" t="s">
         <v>568</v>
       </c>
-      <c r="T112" s="0" t="s">
+      <c r="U112" s="0" t="s">
         <v>569</v>
       </c>
-      <c r="U112" s="0" t="s">
+      <c r="V112" s="0" t="s">
         <v>570</v>
       </c>
-      <c r="V112" s="0" t="s">
+      <c r="W112" s="0" t="s">
         <v>571</v>
       </c>
-      <c r="W112" s="0" t="s">
+      <c r="X112" s="0" t="s">
         <v>572</v>
-      </c>
-      <c r="X112" s="0" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="C113" s="7" t="s">
         <v>574</v>
       </c>
-      <c r="B113" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="C113" s="7" t="s">
+      <c r="D113" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E113" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="D113" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="E113" s="7" t="s">
+      <c r="F113" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="F113" s="7" t="s">
-        <v>577</v>
-      </c>
       <c r="G113" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H113" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J113" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="K113" s="7" t="s">
         <v>578</v>
-      </c>
-      <c r="K113" s="7" t="s">
-        <v>579</v>
       </c>
       <c r="L113" s="7"/>
       <c r="M113" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="N113" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="N113" s="7" t="s">
+      <c r="O113" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="O113" s="7" t="s">
-        <v>582</v>
-      </c>
       <c r="P113" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="Q113" s="7" t="n">
         <v>0</v>
@@ -9637,13 +9355,13 @@
         <v>0</v>
       </c>
       <c r="T113" s="0" t="s">
+        <v>582</v>
+      </c>
+      <c r="U113" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="U113" s="0" t="s">
+      <c r="V113" s="0" t="s">
         <v>584</v>
-      </c>
-      <c r="V113" s="0" t="s">
-        <v>585</v>
       </c>
       <c r="W113" s="0" t="n">
         <v>0</v>
@@ -9654,7 +9372,7 @@
     </row>
     <row r="114" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
@@ -9678,7 +9396,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>94</v>
@@ -9752,7 +9470,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>94</v>
@@ -9826,7 +9544,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>94</v>
@@ -9900,7 +9618,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="7" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>94</v>
@@ -9974,7 +9692,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="7" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>94</v>
@@ -10048,7 +9766,7 @@
     </row>
     <row r="120" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
@@ -10072,7 +9790,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>94</v>
@@ -10081,7 +9799,7 @@
         <v>17</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E121" s="1" t="n">
         <v>154</v>
@@ -10090,13 +9808,13 @@
         <v>14</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H121" s="1" t="n">
         <v>7</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J121" s="1" t="n">
         <v>26</v>
@@ -10105,7 +9823,7 @@
         <v>19</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M121" s="1" t="n">
         <v>8</v>
@@ -10114,10 +9832,10 @@
         <v>57</v>
       </c>
       <c r="O121" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q121" s="1" t="n">
         <v>0</v>
@@ -10146,31 +9864,31 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E122" s="1" t="n">
         <v>74</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H122" s="1" t="n">
         <v>8</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J122" s="1" t="n">
         <v>15</v>
@@ -10179,7 +9897,7 @@
         <v>14</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M122" s="1" t="n">
         <v>4</v>
@@ -10188,10 +9906,10 @@
         <v>28</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q122" s="1" t="n">
         <v>0</v>
@@ -10220,31 +9938,31 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E123" s="1" t="n">
         <v>39</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H123" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J123" s="1" t="n">
         <v>10</v>
@@ -10253,7 +9971,7 @@
         <v>6</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M123" s="1" t="n">
         <v>2</v>
@@ -10262,10 +9980,10 @@
         <v>8</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q123" s="1" t="n">
         <v>0</v>
@@ -10294,7 +10012,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>94</v>
@@ -10303,7 +10021,7 @@
         <v>11</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E124" s="1" t="n">
         <v>3</v>
@@ -10312,13 +10030,13 @@
         <v>1</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H124" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J124" s="1" t="n">
         <v>0</v>
@@ -10327,7 +10045,7 @@
         <v>6</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M124" s="1" t="n">
         <v>2</v>
@@ -10336,10 +10054,10 @@
         <v>1</v>
       </c>
       <c r="O124" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q124" s="1" t="n">
         <v>0</v>
@@ -10368,7 +10086,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>94</v>
@@ -10377,7 +10095,7 @@
         <v>303</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E125" s="1" t="n">
         <v>39</v>
@@ -10386,13 +10104,13 @@
         <v>30</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H125" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J125" s="1" t="n">
         <v>0</v>
@@ -10401,7 +10119,7 @@
         <v>54</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="M125" s="1" t="n">
         <v>20</v>
@@ -10410,10 +10128,10 @@
         <v>110</v>
       </c>
       <c r="O125" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Q125" s="1" t="n">
         <v>0</v>
@@ -10442,12 +10160,12 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O126" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E127" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
   </sheetData>
@@ -10468,39 +10186,39 @@
     <hyperlink ref="U18" r:id="rId14" display="https://github.com/espressomd/espresso"/>
     <hyperlink ref="V18" r:id="rId15" display="https://github.com/espressopp/espressopp"/>
     <hyperlink ref="W18" r:id="rId16" display="https://github.com/UCL/hemelb"/>
-    <hyperlink ref="J20" r:id="rId17" display="https://github.com/aharwood2/LUMA/wiki/Performance"/>
+    <hyperlink ref="J20" r:id="rId17" display="yes, parallelism among other things described in https://github.com/aharwood2/LUMA/wiki/Performance"/>
     <hyperlink ref="W20" r:id="rId18" display="yes, performance mentioned in original publication (linked from repo - https://doi.org/10.1016/j.cpc.2008.02.013)"/>
-    <hyperlink ref="J30" r:id="rId19" display="https://github.com/aharwood2/LUMA/wiki/Validation"/>
+    <hyperlink ref="J30" r:id="rId19" display="yes, installation has a command to run the program; there is also https://github.com/aharwood2/LUMA/wiki/Validation"/>
     <hyperlink ref="S38" r:id="rId20" display="lots of packages need to be manually installed: https://travis-ci.org/github/UCL/LatBo.jl"/>
-    <hyperlink ref="C40" r:id="rId21" display="https://walberla.net/index.html"/>
-    <hyperlink ref="D40" r:id="rId22" display="http://sunlightlb.sourceforge.net/"/>
-    <hyperlink ref="E40" r:id="rId23" location="academic-papers" display="http://sailfish.us.edu.pl/media.html#academic-papers"/>
-    <hyperlink ref="J40" r:id="rId24" display="https://github.com/aharwood2/LUMA/wiki"/>
+    <hyperlink ref="C40" r:id="rId21" display="yes, some theory in publications and documentations on https://walberla.net/index.html"/>
+    <hyperlink ref="D40" r:id="rId22" display="yes, http://sunlightlb.sourceforge.net/"/>
+    <hyperlink ref="E40" r:id="rId23" location="academic-papers" display="yes, http://sailfish.us.edu.pl/media.html#academic-papers"/>
+    <hyperlink ref="J40" r:id="rId24" display="yes, link to https://github.com/aharwood2/LUMA/wiki"/>
     <hyperlink ref="K40" r:id="rId25" display="yes, reference document https://github.com/ludwig-cf/ludwig/blob/master/docs/references.tex"/>
     <hyperlink ref="M40" r:id="rId26" display="yes, some requirements in https://github.com/Olllom/lettuce/blob/master/requirements_dev.txt"/>
     <hyperlink ref="N40" r:id="rId27" display="yes, references to theory in https://pylbm.readthedocs.io/en/latest/"/>
     <hyperlink ref="W40" r:id="rId28" display="yes, theory mentioned in original publication (linked from repo – https://doi.org/10.1016/j.cpc.2008.02.013), as well as in the documentation file"/>
-    <hyperlink ref="F66" r:id="rId29" display="https://palabos.unige.ch/"/>
+    <hyperlink ref="F66" r:id="rId29" display="yes, in https://palabos.unige.ch/"/>
     <hyperlink ref="K69" r:id="rId30" display="considering https://ludwig.epcc.ed.ac.uk/index.html as user manual"/>
-    <hyperlink ref="C72" r:id="rId31" display="https://i10git.cs.fau.de/walberla/walberla"/>
-    <hyperlink ref="E72" r:id="rId32" location="development-team" display="http://sailfish.us.edu.pl/about.html#development-team"/>
-    <hyperlink ref="F72" r:id="rId33" display="https://gitlab.com/unigespc/palabos/blob/master/CONTRIBUTING.md"/>
+    <hyperlink ref="C72" r:id="rId31" display="yes, https://i10git.cs.fau.de/walberla/walberla"/>
+    <hyperlink ref="E72" r:id="rId32" location="development-team" display="yes, http://sailfish.us.edu.pl/about.html#development-team"/>
+    <hyperlink ref="F72" r:id="rId33" display="yes, https://gitlab.com/unigespc/palabos/blob/master/CONTRIBUTING.md"/>
     <hyperlink ref="K72" r:id="rId34" display="yes, https://github.com/ludwig-cf/ludwig/blob/master/CONTRIBUTING.md"/>
     <hyperlink ref="M72" r:id="rId35" display="yes, there is a contributing page https://github.com/Olllom/lettuce/blob/master/CONTRIBUTING.rst"/>
     <hyperlink ref="M84" r:id="rId36" display="api: https://github.com/Olllom/lettuce/blob/master/docs/modules.rst"/>
-    <hyperlink ref="J87" r:id="rId37" display="https://github.com/aharwood2/LUMA/blob/master/LUMA/docs/LUMA%20Coding%20Standards.pdf"/>
+    <hyperlink ref="J87" r:id="rId37" display="yes, https://github.com/aharwood2/LUMA/blob/master/LUMA/docs/LUMA%20Coding%20Standards.pdf"/>
     <hyperlink ref="K97" r:id="rId38" display="yes, README links to https://nvie.com/posts/a-successful-git-branching-model/, but the model is not given a name"/>
-    <hyperlink ref="F98" r:id="rId39" display="https://gitlab.com/unigespc/palabos/-/blob/master/CONTRIBUTING.md"/>
+    <hyperlink ref="F98" r:id="rId39" display="yes, https://gitlab.com/unigespc/palabos/-/blob/master/CONTRIBUTING.md"/>
     <hyperlink ref="K98" r:id="rId40" display="yes, in https://github.com/ludwig-cf/ludwig/blob/master/CONTRIBUTING.md"/>
     <hyperlink ref="N98" r:id="rId41" display="yes, status is “3 – Alpha” on https://pypi.org/project/pylbm/"/>
     <hyperlink ref="O98" r:id="rId42" display="yes, status is “4 – Beta” on https://pypi.org/project/lbmpy/"/>
     <hyperlink ref="L99" r:id="rId43" display="yes, commented https://code.google.com/archive/p/limbes/wikis/QuickStart.wiki"/>
     <hyperlink ref="M99" r:id="rId44" display="yes, requirements are found at https://github.com/Olllom/lettuce/blob/master/requirements_dev.txt"/>
     <hyperlink ref="S99" r:id="rId45" display="yes, clearly laid out in https://travis-ci.org/github/UCL/LatBo.jl (very good)"/>
-    <hyperlink ref="E100" r:id="rId46" display="http://sailfish.us.edu.pl/release.html"/>
-    <hyperlink ref="F100" r:id="rId47" display="https://gitlab.com/unigespc/palabos/-/blob/master/CHANGELOG.md"/>
-    <hyperlink ref="H100" r:id="rId48" display="https://github.com/carlosrosales/mplabs/blob/master/CHANGES.TXT"/>
-    <hyperlink ref="J100" r:id="rId49" display="https://github.com/aharwood2/LUMA/wiki/Release-Notes"/>
+    <hyperlink ref="E100" r:id="rId46" display="yes, http://sailfish.us.edu.pl/release.html"/>
+    <hyperlink ref="F100" r:id="rId47" display="yes, https://gitlab.com/unigespc/palabos/-/blob/master/CHANGELOG.md"/>
+    <hyperlink ref="H100" r:id="rId48" display="yes, https://github.com/carlosrosales/mplabs/blob/master/CHANGES.TXT"/>
+    <hyperlink ref="J100" r:id="rId49" display="yes, https://github.com/aharwood2/LUMA/wiki/Release-Notes"/>
     <hyperlink ref="M102" r:id="rId50" display="there is info on contributing to development at https://github.com/Olllom/lettuce/blob/master/CONTRIBUTING.rst"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fixed overall impression error in completed measures, and adding file documenting how impression was calculated
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -2033,7 +2033,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2099,22 +2099,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2149,13 +2133,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="V91" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
-      <selection pane="topRight" activeCell="W102" activeCellId="0" sqref="W102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -3956,299 +3940,299 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" s="18" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="E28" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="I28" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="J28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="L28" s="16" t="s">
+      <c r="L28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="M28" s="16" t="s">
+      <c r="M28" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="N28" s="16" t="s">
+      <c r="N28" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="O28" s="16" t="s">
+      <c r="O28" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="P28" s="16" t="s">
+      <c r="P28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="Q28" s="16" t="s">
+      <c r="Q28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="R28" s="16" t="s">
+      <c r="R28" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="S28" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="T28" s="17" t="s">
+      <c r="S28" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T28" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="U28" s="17" t="s">
+      <c r="U28" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="V28" s="17" t="s">
+      <c r="V28" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="W28" s="17" t="s">
+      <c r="W28" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="X28" s="17" t="s">
+      <c r="X28" s="15" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" s="17" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="s">
+    <row r="29" s="15" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" s="16" t="s">
+      <c r="C29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="G29" s="16" t="s">
+      <c r="G29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="16" t="s">
+      <c r="H29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="J29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="L29" s="16" t="s">
+      <c r="J29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="L29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="M29" s="16" t="s">
+      <c r="M29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="N29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="O29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="P29" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q29" s="16" t="s">
+      <c r="N29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="R29" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="S29" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="T29" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="U29" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="V29" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="W29" s="17" t="s">
-        <v>229</v>
-      </c>
-      <c r="X29" s="17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" s="18" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
+      <c r="R29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" s="16" t="s">
+      <c r="C30" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="I30" s="16" t="s">
+      <c r="I30" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J30" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="K30" s="16" t="s">
+      <c r="K30" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="L30" s="16" t="s">
+      <c r="L30" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="M30" s="16" t="s">
+      <c r="M30" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="N30" s="16" t="s">
+      <c r="N30" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="O30" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="P30" s="16" t="s">
+      <c r="O30" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="P30" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="Q30" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="R30" s="16" t="s">
+      <c r="Q30" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="R30" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="S30" s="16" t="s">
+      <c r="S30" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="T30" s="17" t="s">
+      <c r="T30" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="U30" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="V30" s="16" t="s">
+      <c r="U30" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="V30" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="W30" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="X30" s="17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" s="18" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
+      <c r="W30" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="X30" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C31" s="16" t="n">
+      <c r="C31" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="D31" s="16" t="n">
+      <c r="D31" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="E31" s="16" t="n">
+      <c r="E31" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F31" s="16" t="n">
+      <c r="F31" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G31" s="16" t="n">
+      <c r="G31" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="16" t="n">
+      <c r="H31" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="I31" s="16" t="n">
+      <c r="I31" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="J31" s="16" t="n">
+      <c r="J31" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="K31" s="16" t="n">
+      <c r="K31" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="L31" s="16" t="n">
+      <c r="L31" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="M31" s="16" t="n">
+      <c r="M31" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="N31" s="16" t="n">
+      <c r="N31" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="O31" s="16" t="s">
+      <c r="O31" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="P31" s="16" t="n">
+      <c r="P31" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="Q31" s="16" t="n">
+      <c r="Q31" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="R31" s="16" t="s">
+      <c r="R31" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="S31" s="16" t="s">
+      <c r="S31" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="T31" s="17" t="s">
+      <c r="T31" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="U31" s="17" t="s">
+      <c r="U31" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="V31" s="17" t="s">
+      <c r="V31" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="W31" s="17" t="s">
+      <c r="W31" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="X31" s="17" t="s">
+      <c r="X31" s="15" t="s">
         <v>266</v>
       </c>
     </row>
@@ -5897,13 +5881,13 @@
         <v>287</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="1" t="n">
         <v>10</v>
@@ -5912,7 +5896,7 @@
         <v>10</v>
       </c>
       <c r="H56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" s="1" t="n">
         <v>10</v>
@@ -5933,19 +5917,19 @@
         <v>10</v>
       </c>
       <c r="O56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S56" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T56" s="0" t="n">
         <v>10</v>
@@ -5957,7 +5941,7 @@
         <v>7</v>
       </c>
       <c r="W56" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X56" s="0" t="n">
         <v>10</v>
@@ -6793,10 +6777,10 @@
       <c r="T71" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="U71" s="20" t="s">
+      <c r="U71" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="V71" s="20" t="s">
+      <c r="V71" s="16" t="s">
         <v>431</v>
       </c>
       <c r="W71" s="0" t="s">
@@ -7035,40 +7019,40 @@
       <c r="B75" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C75" s="21" t="n">
+      <c r="C75" s="17" t="n">
         <v>0.729</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="E75" s="21" t="n">
+      <c r="E75" s="17" t="n">
         <v>0.2222</v>
       </c>
-      <c r="F75" s="21" t="n">
+      <c r="F75" s="17" t="n">
         <v>0.8947</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="H75" s="21" t="n">
+      <c r="H75" s="17" t="n">
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="J75" s="21" t="n">
+      <c r="J75" s="17" t="n">
         <v>0.8571</v>
       </c>
-      <c r="K75" s="21" t="n">
+      <c r="K75" s="17" t="n">
         <v>0.6</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="M75" s="21" t="n">
+      <c r="M75" s="17" t="n">
         <v>0.3333</v>
       </c>
-      <c r="N75" s="21" t="n">
+      <c r="N75" s="17" t="n">
         <v>0.6666</v>
       </c>
       <c r="O75" s="1" t="s">
@@ -7083,22 +7067,22 @@
       <c r="R75" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="S75" s="21" t="n">
+      <c r="S75" s="17" t="n">
         <v>0.9333</v>
       </c>
-      <c r="T75" s="22" t="n">
+      <c r="T75" s="18" t="n">
         <v>0.6032</v>
       </c>
-      <c r="U75" s="22" t="n">
+      <c r="U75" s="18" t="n">
         <v>0.8926</v>
       </c>
-      <c r="V75" s="22" t="n">
+      <c r="V75" s="18" t="n">
         <v>0.6628</v>
       </c>
       <c r="W75" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="X75" s="22" t="n">
+      <c r="X75" s="18" t="n">
         <v>0.1875</v>
       </c>
     </row>
@@ -7109,73 +7093,73 @@
       <c r="B76" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="C76" s="23" t="n">
+      <c r="C76" s="19" t="n">
         <v>0.2262</v>
       </c>
-      <c r="D76" s="23" t="n">
+      <c r="D76" s="19" t="n">
         <v>0.1767</v>
       </c>
-      <c r="E76" s="23" t="n">
+      <c r="E76" s="19" t="n">
         <v>0.0926</v>
       </c>
-      <c r="F76" s="23" t="n">
+      <c r="F76" s="19" t="n">
         <v>0.1776</v>
       </c>
-      <c r="G76" s="23" t="n">
+      <c r="G76" s="19" t="n">
         <v>0.2243</v>
       </c>
-      <c r="H76" s="23" t="n">
+      <c r="H76" s="19" t="n">
         <v>0.2667</v>
       </c>
-      <c r="I76" s="23" t="n">
+      <c r="I76" s="19" t="n">
         <v>0.1511</v>
       </c>
-      <c r="J76" s="23" t="n">
+      <c r="J76" s="19" t="n">
         <v>0.002</v>
       </c>
-      <c r="K76" s="23" t="n">
+      <c r="K76" s="19" t="n">
         <v>0.207</v>
       </c>
-      <c r="L76" s="23" t="n">
+      <c r="L76" s="19" t="n">
         <v>0.1739</v>
       </c>
-      <c r="M76" s="23" t="n">
+      <c r="M76" s="19" t="n">
         <v>0.0819</v>
       </c>
-      <c r="N76" s="23" t="n">
+      <c r="N76" s="19" t="n">
         <v>0.1612</v>
       </c>
-      <c r="O76" s="23" t="n">
+      <c r="O76" s="19" t="n">
         <v>0.0203</v>
       </c>
-      <c r="P76" s="23" t="n">
+      <c r="P76" s="19" t="n">
         <v>0.1376</v>
       </c>
-      <c r="Q76" s="23" t="n">
+      <c r="Q76" s="19" t="n">
         <v>0.1361</v>
       </c>
-      <c r="R76" s="23" t="n">
+      <c r="R76" s="19" t="n">
         <v>0.1434</v>
       </c>
-      <c r="S76" s="23" t="n">
+      <c r="S76" s="19" t="n">
         <v>0.004</v>
       </c>
-      <c r="T76" s="22" t="n">
+      <c r="T76" s="18" t="n">
         <v>0.0602</v>
       </c>
-      <c r="U76" s="22" t="n">
+      <c r="U76" s="18" t="n">
         <v>0.2178</v>
       </c>
-      <c r="V76" s="22" t="n">
+      <c r="V76" s="18" t="n">
         <v>0.171</v>
       </c>
-      <c r="W76" s="22" t="n">
+      <c r="W76" s="18" t="n">
         <v>0.1668</v>
       </c>
-      <c r="X76" s="22" t="n">
+      <c r="X76" s="18" t="n">
         <v>0.0247</v>
       </c>
-      <c r="AB76" s="22"/>
+      <c r="AB76" s="18"/>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">

</xml_diff>

<commit_message>
updated LBM measurements, fixed constants question and answers - updated notes to yes answer
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="610">
   <si>
     <t xml:space="preserve">Metrics &amp; Description</t>
   </si>
@@ -1613,7 +1613,40 @@
     <t xml:space="preserve">Are constants (other than 0 and 1) hard coded into the program? </t>
   </si>
   <si>
-    <t xml:space="preserve">no, did not see any in 10 files</t>
+    <t xml:space="preserve">({yes*, no , unclear})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, grid weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, buffer size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, collision parameters – vague variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, collision neighbours, iterations in examples, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, matrices definitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, velocity directions, limits of planes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, matrices, gradients (fluid, other), unclear tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, matrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, epsilon, pi, blood parameters, matrices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, iterations, Avogadro constant, Boltzmann constant in Joule per Kelvin</t>
   </si>
   <si>
     <t xml:space="preserve">Comments are clear, indicate what is being done, not how?</t>
@@ -2034,7 +2067,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2123,6 +2156,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2142,16 +2187,16 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="R80" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+      <selection pane="topRight" activeCell="Z88" activeCellId="0" sqref="Z88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="1" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.86"/>
@@ -7998,86 +8043,86 @@
         <v>218</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+    <row r="88" s="24" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="22" t="s">
         <v>502</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F88" s="7" t="s">
+      <c r="B88" s="22" t="s">
         <v>503</v>
       </c>
-      <c r="G88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="H88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="I88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="J88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="K88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="L88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="M88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="N88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="O88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="P88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="Q88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="R88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="S88" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="T88" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="U88" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="V88" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="W88" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="X88" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="Y88" s="0" t="s">
-        <v>218</v>
+      <c r="C88" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>506</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G88" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="H88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="I88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="J88" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="K88" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="L88" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="M88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="N88" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="O88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="P88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="R88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="S88" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="T88" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="U88" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="V88" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="W88" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="X88" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="Y88" s="23" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>500</v>
@@ -8154,7 +8199,7 @@
     </row>
     <row r="90" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>505</v>
+        <v>516</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>500</v>
@@ -8163,31 +8208,31 @@
         <v>218</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>218</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>218</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="K90" s="7" t="s">
         <v>218</v>
       </c>
       <c r="L90" s="7" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="M90" s="7" t="s">
         <v>218</v>
@@ -8202,28 +8247,28 @@
         <v>218</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="R90" s="1" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="S90" s="1" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="T90" s="1" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="U90" s="0" t="s">
         <v>218</v>
       </c>
       <c r="V90" s="0" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="W90" s="0" t="s">
         <v>218</v>
       </c>
       <c r="X90" s="0" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="Y90" s="0" t="s">
         <v>218</v>
@@ -8231,7 +8276,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>500</v>
@@ -8255,7 +8300,7 @@
         <v>218</v>
       </c>
       <c r="I91" s="7" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="J91" s="7" t="s">
         <v>218</v>
@@ -8264,10 +8309,10 @@
         <v>218</v>
       </c>
       <c r="L91" s="7" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="M91" s="7" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="N91" s="7" t="s">
         <v>218</v>
@@ -8276,10 +8321,10 @@
         <v>218</v>
       </c>
       <c r="P91" s="7" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="R91" s="7" t="s">
         <v>218</v>
@@ -8291,24 +8336,24 @@
         <v>218</v>
       </c>
       <c r="U91" s="0" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="V91" s="0" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="W91" s="0" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="X91" s="0" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="Y91" s="0" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>500</v>
@@ -8465,27 +8510,27 @@
         <v>213</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="R94" s="7" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="S94" s="1" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
     </row>
     <row r="95" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
@@ -8509,10 +8554,10 @@
     </row>
     <row r="96" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>199</v>
@@ -8542,7 +8587,7 @@
         <v>199</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="M96" s="7" t="s">
         <v>199</v>
@@ -8586,7 +8631,7 @@
     </row>
     <row r="97" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>519</v>
+        <v>530</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>227</v>
@@ -8604,7 +8649,7 @@
         <v>199</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>520</v>
+        <v>531</v>
       </c>
       <c r="H97" s="7" t="s">
         <v>199</v>
@@ -8619,7 +8664,7 @@
         <v>433</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="M97" s="7" t="s">
         <v>199</v>
@@ -8628,10 +8673,10 @@
         <v>199</v>
       </c>
       <c r="O97" s="8" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="Q97" s="7" t="s">
         <v>199</v>
@@ -8646,10 +8691,10 @@
         <v>199</v>
       </c>
       <c r="U97" s="0" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="V97" s="0" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
       <c r="W97" s="0" t="s">
         <v>199</v>
@@ -8663,7 +8708,7 @@
     </row>
     <row r="98" customFormat="false" ht="27.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>526</v>
+        <v>537</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>197</v>
@@ -8684,10 +8729,10 @@
         <v>199</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>527</v>
+        <v>538</v>
       </c>
       <c r="I98" s="7" t="s">
-        <v>528</v>
+        <v>539</v>
       </c>
       <c r="J98" s="7" t="s">
         <v>199</v>
@@ -8699,10 +8744,10 @@
         <v>199</v>
       </c>
       <c r="M98" s="8" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="N98" s="8" t="s">
-        <v>530</v>
+        <v>541</v>
       </c>
       <c r="O98" s="7" t="s">
         <v>199</v>
@@ -8714,13 +8759,13 @@
         <v>199</v>
       </c>
       <c r="R98" s="7" t="s">
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="S98" s="7" t="s">
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="T98" s="8" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="U98" s="0" t="s">
         <v>199</v>
@@ -8732,7 +8777,7 @@
         <v>199</v>
       </c>
       <c r="X98" s="0" t="s">
-        <v>533</v>
+        <v>544</v>
       </c>
       <c r="Y98" s="0" t="s">
         <v>199</v>
@@ -8740,13 +8785,13 @@
     </row>
     <row r="99" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>197</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>429</v>
@@ -8755,25 +8800,25 @@
         <v>199</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>538</v>
+        <v>549</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="J99" s="7" t="s">
         <v>199</v>
       </c>
       <c r="K99" s="8" t="s">
-        <v>540</v>
+        <v>551</v>
       </c>
       <c r="L99" s="7" t="s">
-        <v>541</v>
+        <v>552</v>
       </c>
       <c r="M99" s="7" t="s">
         <v>199</v>
@@ -8899,7 +8944,7 @@
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="7" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -8911,7 +8956,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="8" t="s">
-        <v>543</v>
+        <v>554</v>
       </c>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
@@ -8922,7 +8967,7 @@
     </row>
     <row r="104" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -8939,7 +8984,7 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
       <c r="P104" s="5" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="Q104" s="5"/>
       <c r="R104" s="5"/>
@@ -8948,7 +8993,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>98</v>
@@ -9025,7 +9070,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>98</v>
@@ -9102,7 +9147,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>98</v>
@@ -9179,19 +9224,19 @@
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="D108" s="7" t="n">
         <v>1573654</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="F108" s="7" t="n">
         <v>154310</v>
@@ -9200,13 +9245,13 @@
         <v>727494</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="I108" s="7" t="n">
         <v>192269</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="K108" s="7" t="n">
         <v>10725979</v>
@@ -9215,7 +9260,7 @@
         <v>2252783</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="N108" s="7" t="n">
         <v>6322</v>
@@ -9227,7 +9272,7 @@
         <v>89081</v>
       </c>
       <c r="Q108" s="7" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="R108" s="7" t="n">
         <v>16078</v>
@@ -9256,19 +9301,19 @@
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="D109" s="7" t="n">
         <v>297209</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="F109" s="7" t="n">
         <v>71872</v>
@@ -9277,13 +9322,13 @@
         <v>173808</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="I109" s="7" t="n">
         <v>149144</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="K109" s="7" t="n">
         <v>5201357</v>
@@ -9292,7 +9337,7 @@
         <v>1580570</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="N109" s="7" t="n">
         <v>740</v>
@@ -9304,7 +9349,7 @@
         <v>42448</v>
       </c>
       <c r="Q109" s="7" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="R109" s="7" t="n">
         <v>3132</v>
@@ -9333,19 +9378,19 @@
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>553</v>
+        <v>564</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="D110" s="7" t="n">
         <v>1314</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="F110" s="7" t="n">
         <v>1846</v>
@@ -9354,13 +9399,13 @@
         <v>132</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="I110" s="7" t="n">
         <v>11</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="K110" s="7" t="n">
         <v>697</v>
@@ -9369,7 +9414,7 @@
         <v>2059</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="N110" s="7" t="n">
         <v>50</v>
@@ -9381,7 +9426,7 @@
         <v>488</v>
       </c>
       <c r="Q110" s="7" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="R110" s="7" t="n">
         <v>14</v>
@@ -9410,55 +9455,55 @@
     </row>
     <row r="111" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>556</v>
+        <v>567</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="I111" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>559</v>
+        <v>570</v>
       </c>
       <c r="L111" s="7" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="N111" s="7" t="s">
-        <v>561</v>
+        <v>572</v>
       </c>
       <c r="O111" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="P111" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q111" s="7" t="s">
         <v>562</v>
-      </c>
-      <c r="P111" s="7" t="s">
-        <v>563</v>
-      </c>
-      <c r="Q111" s="7" t="s">
-        <v>551</v>
       </c>
       <c r="R111" s="7" t="n">
         <v>0</v>
@@ -9467,73 +9512,73 @@
         <v>0</v>
       </c>
       <c r="T111" s="7" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="U111" s="0" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="V111" s="0" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="W111" s="0" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
       <c r="X111" s="0" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="Y111" s="0" t="s">
-        <v>569</v>
+        <v>580</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>570</v>
+        <v>581</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>573</v>
+        <v>584</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="I112" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="L112" s="7" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="M112" s="7"/>
       <c r="N112" s="7" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="O112" s="7" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="P112" s="7" t="s">
-        <v>578</v>
+        <v>589</v>
       </c>
       <c r="Q112" s="7" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="R112" s="7" t="n">
         <v>0</v>
@@ -9545,13 +9590,13 @@
         <v>0</v>
       </c>
       <c r="U112" s="0" t="s">
-        <v>579</v>
+        <v>590</v>
       </c>
       <c r="V112" s="0" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="W112" s="0" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="X112" s="0" t="n">
         <v>0</v>
@@ -9562,7 +9607,7 @@
     </row>
     <row r="113" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>582</v>
+        <v>593</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -9586,7 +9631,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>98</v>
@@ -9663,7 +9708,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>583</v>
+        <v>594</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>98</v>
@@ -9740,7 +9785,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>584</v>
+        <v>595</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>98</v>
@@ -9817,7 +9862,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>98</v>
@@ -9894,7 +9939,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>98</v>
@@ -9971,7 +10016,7 @@
     </row>
     <row r="119" s="6" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
@@ -9995,10 +10040,10 @@
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>588</v>
+        <v>599</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>234</v>
@@ -10040,7 +10085,7 @@
         <v>57</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="Q120" s="1" t="s">
         <v>234</v>
@@ -10072,10 +10117,10 @@
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>234</v>
@@ -10117,7 +10162,7 @@
         <v>28</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="Q121" s="1" t="s">
         <v>234</v>
@@ -10149,10 +10194,10 @@
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>234</v>
@@ -10194,7 +10239,7 @@
         <v>8</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>594</v>
+        <v>605</v>
       </c>
       <c r="Q122" s="1" t="s">
         <v>234</v>
@@ -10226,10 +10271,10 @@
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>595</v>
+        <v>606</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>234</v>
@@ -10271,7 +10316,7 @@
         <v>1</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="Q123" s="1" t="s">
         <v>234</v>
@@ -10303,10 +10348,10 @@
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>596</v>
+        <v>607</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>234</v>
@@ -10348,7 +10393,7 @@
         <v>110</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="Q124" s="1" t="s">
         <v>234</v>
@@ -10380,12 +10425,12 @@
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P125" s="1" t="s">
-        <v>597</v>
+        <v>608</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F126" s="1" t="s">
-        <v>598</v>
+        <v>609</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed error in LBM measurement template
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Peter-Notes/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -2176,14 +2176,14 @@
   <dimension ref="A1:AC127"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
-      <selection pane="bottomRight" activeCell="Y34" activeCellId="0" sqref="Y34"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -4051,7 +4051,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>226</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>228</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>228</v>
@@ -4744,7 +4744,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>276</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>7</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>9</v>

</xml_diff>